<commit_message>
Meeting Recording & Burndown
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 4.xlsx
+++ b/Documents/Agile Documents/Burndown Charts/Burndown - Sprint 4.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2cartj31\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\Burndown Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88B6B79-052C-4AF2-A9BE-9E8B7C2FEC46}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -304,7 +305,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -447,16 +447,16 @@
                   <c:v>37.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.75</c:v>
+                  <c:v>25.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.75</c:v>
+                  <c:v>25.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.75</c:v>
+                  <c:v>25.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.75</c:v>
+                  <c:v>25.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,7 +597,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -605,6 +604,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1519,7 +1519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1571,19 +1571,19 @@
       </c>
       <c r="E3" s="2">
         <f>$C3-SUM(C7:D38)</f>
-        <v>37.75</v>
+        <v>25.75</v>
       </c>
       <c r="F3" s="2">
         <f>$C3-SUM(C7:E38)</f>
-        <v>37.75</v>
+        <v>25.75</v>
       </c>
       <c r="G3" s="2">
         <f>$C3-SUM(C7:F38)</f>
-        <v>37.75</v>
+        <v>25.75</v>
       </c>
       <c r="H3" s="2">
         <f>$C3-SUM(C7:G38)</f>
-        <v>37.75</v>
+        <v>25.75</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1655,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="8">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
@@ -1705,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="8">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
@@ -1780,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -1880,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16" s="8">
         <v>0</v>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19" s="8">
         <v>0</v>
@@ -2005,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="8">
         <v>0</v>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="8">
         <v>0</v>

</xml_diff>